<commit_message>
Completed Inserting and Deleting Rows and Columns
</commit_message>
<xml_diff>
--- a/05 - Modifying an Excel Worksheet/MonthlyBudget.xlsx
+++ b/05 - Modifying an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/05 - Modifying an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3F387EB-6192-41C1-8BCE-0129ABD8D3FB}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C94ACD6A-91CD-4156-9891-9E877078F984}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>COUNT</t>
+  </si>
+  <si>
+    <t>Water</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G15"/>
+  <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -407,15 +410,15 @@
     <col min="1" max="1" width="12.26953125" customWidth="1"/>
     <col min="2" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -428,14 +431,17 @@
       <c r="E4" s="1">
         <v>42795</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1">
+        <v>42826</v>
+      </c>
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -449,15 +455,18 @@
         <v>1000</v>
       </c>
       <c r="F5">
-        <f>SUM(C5:E5)</f>
-        <v>3400</v>
+        <v>900</v>
       </c>
       <c r="G5">
-        <f>F5/$F$10</f>
-        <v>0.62442607897153357</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+        <f>SUM(C5:F5)</f>
+        <v>4300</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H11" si="0">G5/$G$11</f>
+        <v>0.58623040218132239</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -471,15 +480,18 @@
         <v>100</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F9" si="0">SUM(C6:E6)</f>
-        <v>335</v>
+        <v>200</v>
       </c>
       <c r="G6">
-        <f>F6/$F$10</f>
-        <v>6.1524334251606978E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+        <f>SUM(C6:F6)</f>
+        <v>535</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>7.2937968643490114E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -493,155 +505,193 @@
         <v>125</v>
       </c>
       <c r="F7">
+        <v>150</v>
+      </c>
+      <c r="G7">
+        <f>SUM(C7:F7)</f>
+        <v>625</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>475</v>
-      </c>
-      <c r="G7">
-        <f>F7/$F$10</f>
-        <v>8.7235996326905416E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+        <v>8.5207907293796861E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>70</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <f>SUM(C8:F8)</f>
+        <v>190</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>2.5903203817314247E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>300</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>275</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>350</v>
       </c>
-      <c r="F8">
+      <c r="F9">
+        <v>300</v>
+      </c>
+      <c r="G9">
+        <f>SUM(C9:F9)</f>
+        <v>1225</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
-        <v>925</v>
-      </c>
-      <c r="G8">
-        <f>F8/$F$10</f>
-        <v>0.16988062442607896</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+        <v>0.16700749829584186</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>100</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>100</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>110</v>
       </c>
-      <c r="F9">
+      <c r="F10">
+        <v>150</v>
+      </c>
+      <c r="G10">
+        <f>SUM(C10:F10)</f>
+        <v>460</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
-        <v>310</v>
-      </c>
-      <c r="G9">
-        <f>F9/$F$10</f>
-        <v>5.6932966023875112E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+        <v>6.2713019768234499E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C10">
-        <f>SUM(C5:C9)</f>
-        <v>1850</v>
-      </c>
-      <c r="D10">
-        <f t="shared" ref="D10:E10" si="1">SUM(D5:D9)</f>
-        <v>1910</v>
-      </c>
-      <c r="E10">
+      <c r="C11">
+        <f>SUM(C5:C10)</f>
+        <v>1900</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:F11" si="1">SUM(D5:D10)</f>
+        <v>1950</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="1"/>
-        <v>1685</v>
-      </c>
-      <c r="F10">
-        <f>SUM(C10:E10)</f>
-        <v>5445</v>
-      </c>
-      <c r="G10">
-        <f>F10/$F$10</f>
+        <v>1755</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>1730</v>
+      </c>
+      <c r="G11">
+        <f>SUM(C11:F11)</f>
+        <v>7335</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="C12">
-        <f>MIN(C5:C9)</f>
-        <v>100</v>
-      </c>
-      <c r="D12">
-        <f t="shared" ref="D12:E12" si="2">MIN(D5:D9)</f>
-        <v>100</v>
-      </c>
-      <c r="E12">
+      <c r="C13">
+        <f>MIN(C5:C10)</f>
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:E13" si="2">MIN(D5:D10)</f>
+        <v>40</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C13">
-        <f>MAX(C5:C9)</f>
+      <c r="C14">
+        <f>MAX(C5:C10)</f>
         <v>1200</v>
       </c>
-      <c r="D13">
-        <f t="shared" ref="D13:E13" si="3">MAX(D5:D9)</f>
+      <c r="D14">
+        <f t="shared" ref="D14:E14" si="3">MAX(D5:D10)</f>
         <v>1200</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <f t="shared" si="3"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C14">
-        <f>AVERAGE(C5:C9)</f>
-        <v>370</v>
-      </c>
-      <c r="D14">
-        <f t="shared" ref="D14:E14" si="4">AVERAGE(D5:D9)</f>
-        <v>382</v>
-      </c>
-      <c r="E14">
+      <c r="C15">
+        <f>AVERAGE(C5:C10)</f>
+        <v>316.66666666666669</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:E15" si="4">AVERAGE(D5:D10)</f>
+        <v>325</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="4"/>
-        <v>337</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+        <v>292.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C15">
-        <f>COUNT(C5:C9)</f>
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <f t="shared" ref="D15:E15" si="5">COUNT(D5:D9)</f>
-        <v>5</v>
-      </c>
-      <c r="E15">
+      <c r="C16">
+        <f>COUNT(C5:C10)</f>
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:E16" si="5">COUNT(D5:D10)</f>
+        <v>6</v>
+      </c>
+      <c r="E16">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C12:E15 C10:E10" formulaRange="1"/>
+    <ignoredError sqref="C13:E16 C11:F11" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>